<commit_message>
updating docs for iteration 2 release
</commit_message>
<xml_diff>
--- a/Doc/CS673_SPPP_RiskManagement_Team4.xlsx
+++ b/Doc/CS673_SPPP_RiskManagement_Team4.xlsx
@@ -10,6 +10,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B7">
+      <text>
+        <t xml:space="preserve">All risks should have some details
+	-Samantha Mott</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G3">
+      <text>
+        <t xml:space="preserve">Using calculations here will make this easier to maintain
+	-Samantha Mott</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="K16">
+      <text>
+        <t xml:space="preserve">If decisions have been made and risk is mitigated, you can keep this updated and mark the items as closed
+	-Samantha Mott</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
   <si>
@@ -310,7 +338,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -321,10 +349,6 @@
     </font>
     <font/>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -413,7 +437,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2098,6 +2122,7 @@
       <c r="AA47" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>